<commit_message>
Read write excel file
</commit_message>
<xml_diff>
--- a/src/test/resources/dataFolder/data.xlsx
+++ b/src/test/resources/dataFolder/data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>firstName</t>
   </si>
@@ -45,12 +45,19 @@
   </si>
   <si>
     <t>Gender</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <sz val="10"/>
@@ -291,15 +298,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -315,8 +322,11 @@
       <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -331,6 +341,9 @@
       </c>
       <c r="E2" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>